<commit_message>
https://kompege.ru/variant?kim=25090569 Task 22 completed
</commit_message>
<xml_diff>
--- a/25-03-25/Task-22.xlsx
+++ b/25-03-25/Task-22.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHohlov\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHohlov\Desktop\EGE\25-03-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4804123C-C049-494E-A7DE-F7534D3FA554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25E5DD6-B4F1-4DCF-B019-EBECD27E8885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -453,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:TS39"/>
+  <dimension ref="A1:TS19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="DK23" sqref="DK23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2073,7 +2069,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="5">
-        <f t="shared" ref="H2:J2" si="0">VLOOKUP(D2,$A:$M,12,0)</f>
+        <f t="shared" ref="H2:I2" si="0">VLOOKUP(D2,$A:$M,12,0)</f>
         <v>0</v>
       </c>
       <c r="I2" s="5">
@@ -2081,31 +2077,31 @@
         <v>0</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" si="0"/>
+        <f>VLOOKUP(F2,$A:$M,12,0)</f>
         <v>0</v>
       </c>
       <c r="K2" s="6">
         <f>L2-B2+1</f>
-        <v>201</v>
+        <v>1</v>
       </c>
       <c r="L2" s="6">
-        <f>MAX(C2:F2)+B2+M2+DK23</f>
-        <v>203</v>
+        <f>MAX(G2:J2)+B2+M2</f>
+        <v>3</v>
       </c>
       <c r="M2" s="7">
-        <v>200</v>
-      </c>
-      <c r="N2" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
         <f>IF(AND($K2&lt;=N$1,N$1&lt;=$L2),1,"")</f>
-        <v/>
-      </c>
-      <c r="O2" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
         <f t="shared" ref="O2:BZ5" si="1">IF(AND($K2&lt;=O$1,O$1&lt;=$L2),1,"")</f>
-        <v/>
-      </c>
-      <c r="P2" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="Q2" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2895,17 +2891,17 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="HF2" s="2">
+      <c r="HF2" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="HG2" s="2">
+        <v/>
+      </c>
+      <c r="HG2" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="HH2" s="2">
+        <v/>
+      </c>
+      <c r="HH2" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="HI2" s="2" t="str">
         <f t="shared" si="4"/>
@@ -4234,7 +4230,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="6">
-        <f t="shared" ref="L3:L18" si="15">MAX(C3:F3)+B3+M3+DK24</f>
+        <f t="shared" ref="L3:L18" si="15">MAX(G3:J3)+B3+M3</f>
         <v>2</v>
       </c>
       <c r="M3" s="7">
@@ -8787,7 +8783,7 @@
         <v/>
       </c>
       <c r="BZ5" s="2" t="str">
-        <f t="shared" ref="O5:BZ18" si="17">IF(AND($K5&lt;=BZ$1,BZ$1&lt;=$L5),1,"")</f>
+        <f t="shared" ref="O5:BZ9" si="17">IF(AND($K5&lt;=BZ$1,BZ$1&lt;=$L5),1,"")</f>
         <v/>
       </c>
       <c r="CA5" s="2" t="str">
@@ -9043,7 +9039,7 @@
         <v/>
       </c>
       <c r="EL5" s="2" t="str">
-        <f t="shared" ref="CA5:EL18" si="18">IF(AND($K5&lt;=EL$1,EL$1&lt;=$L5),1,"")</f>
+        <f t="shared" ref="CA5:EL9" si="18">IF(AND($K5&lt;=EL$1,EL$1&lt;=$L5),1,"")</f>
         <v/>
       </c>
       <c r="EM5" s="2" t="str">
@@ -9299,7 +9295,7 @@
         <v/>
       </c>
       <c r="GX5" s="2" t="str">
-        <f t="shared" ref="EM5:GX18" si="19">IF(AND($K5&lt;=GX$1,GX$1&lt;=$L5),1,"")</f>
+        <f t="shared" ref="EM5:GX9" si="19">IF(AND($K5&lt;=GX$1,GX$1&lt;=$L5),1,"")</f>
         <v/>
       </c>
       <c r="GY5" s="2" t="str">
@@ -9555,7 +9551,7 @@
         <v/>
       </c>
       <c r="JJ5" s="2" t="str">
-        <f t="shared" ref="GY5:JJ18" si="20">IF(AND($K5&lt;=JJ$1,JJ$1&lt;=$L5),1,"")</f>
+        <f t="shared" ref="GY5:JJ9" si="20">IF(AND($K5&lt;=JJ$1,JJ$1&lt;=$L5),1,"")</f>
         <v/>
       </c>
       <c r="JK5" s="2" t="str">
@@ -9811,7 +9807,7 @@
         <v/>
       </c>
       <c r="LV5" s="2" t="str">
-        <f t="shared" ref="JK5:LV18" si="21">IF(AND($K5&lt;=LV$1,LV$1&lt;=$L5),1,"")</f>
+        <f t="shared" ref="JK5:LV9" si="21">IF(AND($K5&lt;=LV$1,LV$1&lt;=$L5),1,"")</f>
         <v/>
       </c>
       <c r="LW5" s="2" t="str">
@@ -10067,7 +10063,7 @@
         <v/>
       </c>
       <c r="OH5" s="2" t="str">
-        <f t="shared" ref="LW5:OH18" si="22">IF(AND($K5&lt;=OH$1,OH$1&lt;=$L5),1,"")</f>
+        <f t="shared" ref="LW5:OH9" si="22">IF(AND($K5&lt;=OH$1,OH$1&lt;=$L5),1,"")</f>
         <v/>
       </c>
       <c r="OI5" s="2" t="str">
@@ -10323,7 +10319,7 @@
         <v/>
       </c>
       <c r="QT5" s="2" t="str">
-        <f t="shared" ref="OI5:QT18" si="23">IF(AND($K5&lt;=QT$1,QT$1&lt;=$L5),1,"")</f>
+        <f t="shared" ref="OI5:QT9" si="23">IF(AND($K5&lt;=QT$1,QT$1&lt;=$L5),1,"")</f>
         <v/>
       </c>
       <c r="QU5" s="2" t="str">
@@ -10579,7 +10575,7 @@
         <v/>
       </c>
       <c r="TF5" s="2" t="str">
-        <f t="shared" ref="QU5:TF18" si="24">IF(AND($K5&lt;=TF$1,TF$1&lt;=$L5),1,"")</f>
+        <f t="shared" ref="QU5:TF9" si="24">IF(AND($K5&lt;=TF$1,TF$1&lt;=$L5),1,"")</f>
         <v/>
       </c>
       <c r="TG5" s="2" t="str">
@@ -10666,11 +10662,11 @@
       </c>
       <c r="K6" s="6">
         <f t="shared" si="14"/>
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" si="15"/>
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="M6" s="7">
         <v>0</v>
@@ -10683,29 +10679,29 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="P6" s="2" t="str">
+      <c r="P6" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="Q6" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="R6" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S6" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="S6" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="T6" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="T6" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="U6" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="U6" s="2">
         <f t="shared" si="17"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="V6" s="2" t="str">
         <f t="shared" si="17"/>
@@ -11083,29 +11079,29 @@
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="DL6" s="2">
+      <c r="DL6" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DM6" s="2">
+        <v/>
+      </c>
+      <c r="DM6" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DN6" s="2">
+        <v/>
+      </c>
+      <c r="DN6" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DO6" s="2">
+        <v/>
+      </c>
+      <c r="DO6" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DP6" s="2">
+        <v/>
+      </c>
+      <c r="DP6" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DQ6" s="2">
+        <v/>
+      </c>
+      <c r="DQ6" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="DR6" s="2" t="str">
         <f t="shared" si="18"/>
@@ -12813,11 +12809,11 @@
       </c>
       <c r="K7" s="6">
         <f t="shared" si="14"/>
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="15"/>
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="M7" s="7">
         <v>0</v>
@@ -12854,37 +12850,37 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="V7" s="2" t="str">
+      <c r="V7" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W7" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="X7" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="Y7" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="Z7" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AA7" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AB7" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AC7" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="2">
         <f t="shared" si="17"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AD7" s="2" t="str">
         <f t="shared" si="17"/>
@@ -13238,37 +13234,37 @@
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="DN7" s="2">
+      <c r="DN7" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DO7" s="2">
+        <v/>
+      </c>
+      <c r="DO7" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DP7" s="2">
+        <v/>
+      </c>
+      <c r="DP7" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DQ7" s="2">
+        <v/>
+      </c>
+      <c r="DQ7" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DR7" s="2">
+        <v/>
+      </c>
+      <c r="DR7" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DS7" s="2">
+        <v/>
+      </c>
+      <c r="DS7" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DT7" s="2">
+        <v/>
+      </c>
+      <c r="DT7" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DU7" s="2">
+        <v/>
+      </c>
+      <c r="DU7" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="DV7" s="2" t="str">
         <f t="shared" si="18"/>
@@ -14942,7 +14938,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5">
         <f t="shared" si="10"/>
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="11"/>
@@ -14958,11 +14954,11 @@
       </c>
       <c r="K8" s="6">
         <f t="shared" si="14"/>
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="15"/>
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="M8" s="7">
         <v>0</v>
@@ -14999,21 +14995,21 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="V8" s="2" t="str">
+      <c r="V8" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W8" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="X8" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="X8" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="Y8" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="2">
         <f t="shared" si="17"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="Z8" s="2" t="str">
         <f t="shared" si="17"/>
@@ -15387,21 +15383,21 @@
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="DO8" s="2">
+      <c r="DO8" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DP8" s="2">
+        <v/>
+      </c>
+      <c r="DP8" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DQ8" s="2">
+        <v/>
+      </c>
+      <c r="DQ8" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DR8" s="2">
+        <v/>
+      </c>
+      <c r="DR8" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="DS8" s="2" t="str">
         <f t="shared" si="18"/>
@@ -17087,7 +17083,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="5">
         <f t="shared" si="10"/>
-        <v>203</v>
+        <v>3</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="11"/>
@@ -17103,11 +17099,11 @@
       </c>
       <c r="K9" s="6">
         <f t="shared" si="14"/>
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="15"/>
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="M9" s="7">
         <v>0</v>
@@ -17124,25 +17120,25 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="Q9" s="2" t="str">
+      <c r="Q9" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="R9" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S9" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="S9" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="T9" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="T9" s="2">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="U9" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="U9" s="2">
         <f t="shared" si="17"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="V9" s="2" t="str">
         <f t="shared" si="17"/>
@@ -17516,25 +17512,25 @@
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="DK9" s="2">
+      <c r="DK9" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DL9" s="2">
+        <v/>
+      </c>
+      <c r="DL9" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DM9" s="2">
+        <v/>
+      </c>
+      <c r="DM9" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DN9" s="2">
+        <v/>
+      </c>
+      <c r="DN9" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="DO9" s="2">
+        <v/>
+      </c>
+      <c r="DO9" s="2" t="str">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="DP9" s="2" t="str">
         <f t="shared" si="18"/>
@@ -19238,27 +19234,27 @@
       </c>
       <c r="G10" s="5">
         <f t="shared" si="10"/>
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="11"/>
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="12"/>
-        <v>112</v>
+        <v>16</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="13"/>
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="14"/>
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="15"/>
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="M10" s="7">
         <v>0</v>
@@ -19327,37 +19323,37 @@
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="AD10" s="2" t="str">
+      <c r="AD10" s="2">
         <f t="shared" ref="AD10:AS18" si="33">IF(AND($K10&lt;=AD$1,AD$1&lt;=$L10),1,"")</f>
-        <v/>
-      </c>
-      <c r="AE10" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AF10" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AG10" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AH10" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AI10" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AJ10" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AK10" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="2">
         <f t="shared" si="33"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AL10" s="2" t="str">
         <f t="shared" si="33"/>
@@ -19695,37 +19691,37 @@
         <f t="shared" si="37"/>
         <v/>
       </c>
-      <c r="DR10" s="2">
+      <c r="DR10" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DS10" s="2">
+        <v/>
+      </c>
+      <c r="DS10" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DT10" s="2">
+        <v/>
+      </c>
+      <c r="DT10" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DU10" s="2">
+        <v/>
+      </c>
+      <c r="DU10" s="2" t="str">
         <f t="shared" ref="DU10:EJ18" si="38">IF(AND($K10&lt;=DU$1,DU$1&lt;=$L10),1,"")</f>
-        <v>1</v>
-      </c>
-      <c r="DV10" s="2">
+        <v/>
+      </c>
+      <c r="DV10" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DW10" s="2">
+        <v/>
+      </c>
+      <c r="DW10" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DX10" s="2">
+        <v/>
+      </c>
+      <c r="DX10" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DY10" s="2">
+        <v/>
+      </c>
+      <c r="DY10" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="DZ10" s="2" t="str">
         <f t="shared" si="38"/>
@@ -21383,7 +21379,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="5">
         <f t="shared" si="10"/>
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="11"/>
@@ -21399,11 +21395,11 @@
       </c>
       <c r="K11" s="6">
         <f t="shared" si="14"/>
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" si="15"/>
-        <v>116</v>
+        <v>21</v>
       </c>
       <c r="M11" s="7">
         <v>0</v>
@@ -21456,41 +21452,41 @@
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="Z11" s="2" t="str">
+      <c r="Z11" s="2">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AA11" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="2">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AB11" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="2">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AC11" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="2">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AD11" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AE11" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AF11" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AG11" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AH11" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="2">
         <f t="shared" si="33"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AI11" s="2" t="str">
         <f t="shared" si="33"/>
@@ -21836,41 +21832,41 @@
         <f t="shared" si="37"/>
         <v/>
       </c>
-      <c r="DQ11" s="2">
+      <c r="DQ11" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DR11" s="2">
+        <v/>
+      </c>
+      <c r="DR11" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DS11" s="2">
+        <v/>
+      </c>
+      <c r="DS11" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DT11" s="2">
+        <v/>
+      </c>
+      <c r="DT11" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DU11" s="2">
+        <v/>
+      </c>
+      <c r="DU11" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DV11" s="2">
+        <v/>
+      </c>
+      <c r="DV11" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DW11" s="2">
+        <v/>
+      </c>
+      <c r="DW11" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DX11" s="2">
+        <v/>
+      </c>
+      <c r="DX11" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DY11" s="2">
+        <v/>
+      </c>
+      <c r="DY11" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="DZ11" s="2" t="str">
         <f t="shared" si="38"/>
@@ -23528,7 +23524,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="5">
         <f t="shared" si="10"/>
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="11"/>
@@ -23544,11 +23540,11 @@
       </c>
       <c r="K12" s="6">
         <f t="shared" si="14"/>
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="15"/>
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="M12" s="7">
         <v>0</v>
@@ -23649,13 +23645,13 @@
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AL12" s="2" t="str">
+      <c r="AL12" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AM12" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="2">
         <f t="shared" si="33"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AN12" s="2" t="str">
         <f t="shared" si="33"/>
@@ -23989,13 +23985,13 @@
         <f t="shared" si="37"/>
         <v/>
       </c>
-      <c r="DS12" s="2">
+      <c r="DS12" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DT12" s="2">
+        <v/>
+      </c>
+      <c r="DT12" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="DU12" s="2" t="str">
         <f t="shared" si="38"/>
@@ -27820,7 +27816,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="5">
         <f t="shared" si="10"/>
-        <v>116</v>
+        <v>21</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="11"/>
@@ -27836,11 +27832,11 @@
       </c>
       <c r="K14" s="6">
         <f t="shared" si="14"/>
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="15"/>
-        <v>118</v>
+        <v>27</v>
       </c>
       <c r="M14" s="7">
         <v>0</v>
@@ -27929,29 +27925,29 @@
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AI14" s="2" t="str">
+      <c r="AI14" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AJ14" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AK14" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AL14" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AM14" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AN14" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="2">
         <f t="shared" si="33"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AO14" s="2" t="str">
         <f t="shared" si="33"/>
@@ -28293,29 +28289,29 @@
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="DV14" s="2">
+      <c r="DV14" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DW14" s="2">
+        <v/>
+      </c>
+      <c r="DW14" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DX14" s="2">
+        <v/>
+      </c>
+      <c r="DX14" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DY14" s="2">
+        <v/>
+      </c>
+      <c r="DY14" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DZ14" s="2">
+        <v/>
+      </c>
+      <c r="DZ14" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EA14" s="2">
+        <v/>
+      </c>
+      <c r="EA14" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="EB14" s="2" t="str">
         <f t="shared" si="38"/>
@@ -29967,11 +29963,11 @@
       <c r="F15" s="4"/>
       <c r="G15" s="5">
         <f t="shared" si="10"/>
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="11"/>
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="12"/>
@@ -29983,11 +29979,11 @@
       </c>
       <c r="K15" s="6">
         <f t="shared" si="14"/>
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="15"/>
-        <v>122</v>
+        <v>34</v>
       </c>
       <c r="M15" s="7">
         <v>0</v>
@@ -30100,33 +30096,33 @@
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AO15" s="2" t="str">
+      <c r="AO15" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AP15" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AQ15" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AQ15" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AR15" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AR15" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AS15" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AS15" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AT15" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AT15" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="AU15" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AU15" s="2">
         <f t="shared" si="34"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AV15" s="2" t="str">
         <f t="shared" si="34"/>
@@ -30452,33 +30448,33 @@
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="DY15" s="2">
+      <c r="DY15" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="DZ15" s="2">
+        <v/>
+      </c>
+      <c r="DZ15" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EA15" s="2">
+        <v/>
+      </c>
+      <c r="EA15" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EB15" s="2">
+        <v/>
+      </c>
+      <c r="EB15" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EC15" s="2">
+        <v/>
+      </c>
+      <c r="EC15" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="ED15" s="2">
+        <v/>
+      </c>
+      <c r="ED15" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EE15" s="2">
+        <v/>
+      </c>
+      <c r="EE15" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="EF15" s="2" t="str">
         <f t="shared" si="38"/>
@@ -32112,7 +32108,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="5">
         <f t="shared" si="10"/>
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="11"/>
@@ -32128,11 +32124,11 @@
       </c>
       <c r="K16" s="6">
         <f t="shared" si="14"/>
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="L16" s="6">
         <f t="shared" si="15"/>
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="M16" s="7">
         <v>0</v>
@@ -32233,17 +32229,17 @@
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="AL16" s="2" t="str">
+      <c r="AL16" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AM16" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="2">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="AN16" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="2">
         <f t="shared" si="33"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="AO16" s="2" t="str">
         <f t="shared" si="33"/>
@@ -32573,17 +32569,17 @@
         <f t="shared" si="37"/>
         <v/>
       </c>
-      <c r="DS16" s="2">
+      <c r="DS16" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DT16" s="2">
+        <v/>
+      </c>
+      <c r="DT16" s="2" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="DU16" s="2">
+        <v/>
+      </c>
+      <c r="DU16" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="DV16" s="2" t="str">
         <f t="shared" si="38"/>
@@ -36404,7 +36400,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="5">
         <f t="shared" si="10"/>
-        <v>122</v>
+        <v>34</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="11"/>
@@ -36420,11 +36416,11 @@
       </c>
       <c r="K18" s="6">
         <f t="shared" si="14"/>
-        <v>117</v>
+        <v>35</v>
       </c>
       <c r="L18" s="6">
         <f t="shared" si="15"/>
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="M18" s="7">
         <v>0</v>
@@ -36565,41 +36561,41 @@
         <f t="shared" si="34"/>
         <v/>
       </c>
-      <c r="AV18" s="2" t="str">
+      <c r="AV18" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="AW18" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AW18" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="AX18" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AX18" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="AY18" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AY18" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="AZ18" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="AZ18" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="BA18" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="BA18" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="BB18" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="BB18" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="BC18" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="BC18" s="2">
         <f t="shared" si="34"/>
-        <v/>
-      </c>
-      <c r="BD18" s="2" t="str">
+        <v>1</v>
+      </c>
+      <c r="BD18" s="2">
         <f t="shared" si="34"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="BE18" s="2" t="str">
         <f t="shared" si="34"/>
@@ -36893,41 +36889,41 @@
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="DZ18" s="2">
+      <c r="DZ18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EA18" s="2">
+        <v/>
+      </c>
+      <c r="EA18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EB18" s="2">
+        <v/>
+      </c>
+      <c r="EB18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EC18" s="2">
+        <v/>
+      </c>
+      <c r="EC18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="ED18" s="2">
+        <v/>
+      </c>
+      <c r="ED18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EE18" s="2">
+        <v/>
+      </c>
+      <c r="EE18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EF18" s="2">
+        <v/>
+      </c>
+      <c r="EF18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EG18" s="2">
+        <v/>
+      </c>
+      <c r="EG18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="EH18" s="2">
+        <v/>
+      </c>
+      <c r="EH18" s="2" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="EI18" s="2" t="str">
         <f t="shared" si="38"/>
@@ -38537,175 +38533,175 @@
     <row r="19" spans="1:539" x14ac:dyDescent="0.35">
       <c r="N19" s="2">
         <f>SUM(N2:N18)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" ref="O19:BZ19" si="57">SUM(O2:O18)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P19" s="2">
         <f t="shared" si="57"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q19" s="2">
         <f t="shared" si="57"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R19" s="2">
         <f t="shared" si="57"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S19" s="2">
         <f t="shared" si="57"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T19" s="2">
         <f t="shared" si="57"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U19" s="2">
         <f t="shared" si="57"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD19" s="2">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE19" s="2">
         <f t="shared" si="57"/>
@@ -38941,99 +38937,99 @@
       </c>
       <c r="DK19" s="2">
         <f t="shared" si="58"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DL19" s="2">
         <f t="shared" si="58"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DM19" s="2">
         <f t="shared" si="58"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DN19" s="2">
         <f t="shared" si="58"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DO19" s="2">
         <f t="shared" si="58"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DP19" s="2">
         <f t="shared" si="58"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DQ19" s="2">
         <f t="shared" si="58"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DR19" s="2">
         <f t="shared" si="58"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DS19" s="2">
         <f t="shared" si="58"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="DT19" s="2">
         <f t="shared" si="58"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="DU19" s="2">
         <f t="shared" si="58"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DV19" s="2">
         <f t="shared" si="58"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DW19" s="2">
         <f t="shared" si="58"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DX19" s="2">
         <f t="shared" si="58"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DY19" s="2">
         <f t="shared" si="58"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DZ19" s="2">
         <f t="shared" si="58"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="EA19" s="2">
         <f t="shared" si="58"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="EB19" s="2">
         <f t="shared" si="58"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="EC19" s="2">
         <f t="shared" si="58"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="ED19" s="2">
         <f t="shared" si="58"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="EE19" s="2">
         <f t="shared" si="58"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="EF19" s="2">
         <f t="shared" si="58"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EG19" s="2">
         <f t="shared" si="58"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EH19" s="2">
         <f t="shared" si="58"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EI19" s="2">
         <f t="shared" si="58"/>
@@ -39337,15 +39333,15 @@
       </c>
       <c r="HF19" s="2">
         <f t="shared" si="60"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HG19" s="2">
         <f t="shared" si="60"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HH19" s="2">
         <f t="shared" si="60"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HI19" s="2">
         <f t="shared" si="60"/>
@@ -40637,728 +40633,6 @@
       </c>
       <c r="TS19" s="2">
         <f t="shared" si="65"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY22" s="1">
-        <v>0</v>
-      </c>
-      <c r="CZ22" s="1">
-        <v>0</v>
-      </c>
-      <c r="DA22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY23" s="1">
-        <v>101</v>
-      </c>
-      <c r="CZ23" s="1">
-        <v>3</v>
-      </c>
-      <c r="DA23" s="3">
-        <v>0</v>
-      </c>
-      <c r="DB23" s="4"/>
-      <c r="DC23" s="4"/>
-      <c r="DD23" s="4"/>
-      <c r="DE23" s="5">
-        <f>VLOOKUP(DA23,$A:$M,12,0)</f>
-        <v>0</v>
-      </c>
-      <c r="DF23" s="5">
-        <f t="shared" ref="DF23:DF39" si="66">VLOOKUP(DB23,$A:$M,12,0)</f>
-        <v>0</v>
-      </c>
-      <c r="DG23" s="5">
-        <f t="shared" ref="DG23:DG39" si="67">VLOOKUP(DC23,$A:$M,12,0)</f>
-        <v>0</v>
-      </c>
-      <c r="DH23" s="5">
-        <f t="shared" ref="DH23:DH39" si="68">VLOOKUP(DD23,$A:$M,12,0)</f>
-        <v>0</v>
-      </c>
-      <c r="DI23" s="6">
-        <f>DJ23-CZ23+1</f>
-        <v>1</v>
-      </c>
-      <c r="DJ23" s="6">
-        <f>MAX(DA23:DD23)+CZ23+DK23+HI44</f>
-        <v>3</v>
-      </c>
-      <c r="DK23" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY24" s="1">
-        <v>102</v>
-      </c>
-      <c r="CZ24" s="1">
-        <v>2</v>
-      </c>
-      <c r="DA24" s="3">
-        <v>0</v>
-      </c>
-      <c r="DB24" s="4"/>
-      <c r="DC24" s="4"/>
-      <c r="DD24" s="4"/>
-      <c r="DE24" s="5">
-        <f t="shared" ref="DE24:DE39" si="69">VLOOKUP(DA24,$A:$M,12,0)</f>
-        <v>0</v>
-      </c>
-      <c r="DF24" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG24" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH24" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI24" s="6">
-        <f t="shared" ref="DI24:DI39" si="70">DJ24-CZ24+1</f>
-        <v>1</v>
-      </c>
-      <c r="DJ24" s="6">
-        <f t="shared" ref="DJ24:DJ39" si="71">MAX(DA24:DD24)+CZ24+DK24+HI45</f>
-        <v>2</v>
-      </c>
-      <c r="DK24" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY25" s="1">
-        <v>103</v>
-      </c>
-      <c r="CZ25" s="1">
-        <v>8</v>
-      </c>
-      <c r="DA25" s="3">
-        <v>0</v>
-      </c>
-      <c r="DB25" s="4"/>
-      <c r="DC25" s="4"/>
-      <c r="DD25" s="4"/>
-      <c r="DE25" s="5">
-        <f t="shared" si="69"/>
-        <v>0</v>
-      </c>
-      <c r="DF25" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG25" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH25" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI25" s="6">
-        <f t="shared" si="70"/>
-        <v>1</v>
-      </c>
-      <c r="DJ25" s="6">
-        <f t="shared" si="71"/>
-        <v>8</v>
-      </c>
-      <c r="DK25" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY26" s="1">
-        <v>104</v>
-      </c>
-      <c r="CZ26" s="1">
-        <v>5</v>
-      </c>
-      <c r="DA26" s="3">
-        <v>0</v>
-      </c>
-      <c r="DB26" s="4"/>
-      <c r="DC26" s="4"/>
-      <c r="DD26" s="4"/>
-      <c r="DE26" s="5">
-        <f t="shared" si="69"/>
-        <v>0</v>
-      </c>
-      <c r="DF26" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG26" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH26" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI26" s="6">
-        <f t="shared" si="70"/>
-        <v>1</v>
-      </c>
-      <c r="DJ26" s="6">
-        <f t="shared" si="71"/>
-        <v>5</v>
-      </c>
-      <c r="DK26" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY27" s="1">
-        <v>105</v>
-      </c>
-      <c r="CZ27" s="1">
-        <v>6</v>
-      </c>
-      <c r="DA27" s="3">
-        <v>102</v>
-      </c>
-      <c r="DB27" s="4"/>
-      <c r="DC27" s="4"/>
-      <c r="DD27" s="4"/>
-      <c r="DE27" s="5">
-        <f t="shared" si="69"/>
-        <v>2</v>
-      </c>
-      <c r="DF27" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG27" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH27" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI27" s="6">
-        <f t="shared" si="70"/>
-        <v>103</v>
-      </c>
-      <c r="DJ27" s="6">
-        <f t="shared" si="71"/>
-        <v>108</v>
-      </c>
-      <c r="DK27" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY28" s="1">
-        <v>106</v>
-      </c>
-      <c r="CZ28" s="1">
-        <v>8</v>
-      </c>
-      <c r="DA28" s="3">
-        <v>103</v>
-      </c>
-      <c r="DB28" s="4">
-        <v>104</v>
-      </c>
-      <c r="DC28" s="4"/>
-      <c r="DD28" s="4"/>
-      <c r="DE28" s="5">
-        <f t="shared" si="69"/>
-        <v>8</v>
-      </c>
-      <c r="DF28" s="5">
-        <f t="shared" si="66"/>
-        <v>5</v>
-      </c>
-      <c r="DG28" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH28" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI28" s="6">
-        <f t="shared" si="70"/>
-        <v>105</v>
-      </c>
-      <c r="DJ28" s="6">
-        <f t="shared" si="71"/>
-        <v>112</v>
-      </c>
-      <c r="DK28" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY29" s="1">
-        <v>107</v>
-      </c>
-      <c r="CZ29" s="1">
-        <v>4</v>
-      </c>
-      <c r="DA29" s="3">
-        <v>105</v>
-      </c>
-      <c r="DB29" s="4"/>
-      <c r="DC29" s="4"/>
-      <c r="DD29" s="4"/>
-      <c r="DE29" s="5">
-        <f t="shared" si="69"/>
-        <v>108</v>
-      </c>
-      <c r="DF29" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG29" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH29" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI29" s="6">
-        <f t="shared" si="70"/>
-        <v>106</v>
-      </c>
-      <c r="DJ29" s="6">
-        <f t="shared" si="71"/>
-        <v>109</v>
-      </c>
-      <c r="DK29" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY30" s="1">
-        <v>108</v>
-      </c>
-      <c r="CZ30" s="1">
-        <v>5</v>
-      </c>
-      <c r="DA30" s="3">
-        <v>101</v>
-      </c>
-      <c r="DB30" s="4"/>
-      <c r="DC30" s="4"/>
-      <c r="DD30" s="4"/>
-      <c r="DE30" s="5">
-        <f t="shared" si="69"/>
-        <v>203</v>
-      </c>
-      <c r="DF30" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG30" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH30" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI30" s="6">
-        <f t="shared" si="70"/>
-        <v>102</v>
-      </c>
-      <c r="DJ30" s="6">
-        <f t="shared" si="71"/>
-        <v>106</v>
-      </c>
-      <c r="DK30" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY31" s="1">
-        <v>109</v>
-      </c>
-      <c r="CZ31" s="1">
-        <v>8</v>
-      </c>
-      <c r="DA31" s="3">
-        <v>108</v>
-      </c>
-      <c r="DB31" s="4">
-        <v>105</v>
-      </c>
-      <c r="DC31" s="4">
-        <v>106</v>
-      </c>
-      <c r="DD31" s="4">
-        <v>107</v>
-      </c>
-      <c r="DE31" s="5">
-        <f t="shared" si="69"/>
-        <v>106</v>
-      </c>
-      <c r="DF31" s="5">
-        <f t="shared" si="66"/>
-        <v>108</v>
-      </c>
-      <c r="DG31" s="5">
-        <f t="shared" si="67"/>
-        <v>112</v>
-      </c>
-      <c r="DH31" s="5">
-        <f t="shared" si="68"/>
-        <v>109</v>
-      </c>
-      <c r="DI31" s="6">
-        <f t="shared" si="70"/>
-        <v>109</v>
-      </c>
-      <c r="DJ31" s="6">
-        <f t="shared" si="71"/>
-        <v>116</v>
-      </c>
-      <c r="DK31" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:539" x14ac:dyDescent="0.35">
-      <c r="CY32" s="1">
-        <v>110</v>
-      </c>
-      <c r="CZ32" s="1">
-        <v>9</v>
-      </c>
-      <c r="DA32" s="3">
-        <v>107</v>
-      </c>
-      <c r="DB32" s="4"/>
-      <c r="DC32" s="4"/>
-      <c r="DD32" s="4"/>
-      <c r="DE32" s="5">
-        <f t="shared" si="69"/>
-        <v>109</v>
-      </c>
-      <c r="DF32" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG32" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH32" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI32" s="6">
-        <f t="shared" si="70"/>
-        <v>108</v>
-      </c>
-      <c r="DJ32" s="6">
-        <f t="shared" si="71"/>
-        <v>116</v>
-      </c>
-      <c r="DK32" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="103:115" x14ac:dyDescent="0.35">
-      <c r="CY33" s="1">
-        <v>111</v>
-      </c>
-      <c r="CZ33" s="1">
-        <v>2</v>
-      </c>
-      <c r="DA33" s="3">
-        <v>109</v>
-      </c>
-      <c r="DB33" s="4"/>
-      <c r="DC33" s="4"/>
-      <c r="DD33" s="4"/>
-      <c r="DE33" s="5">
-        <f t="shared" si="69"/>
-        <v>116</v>
-      </c>
-      <c r="DF33" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG33" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH33" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI33" s="6">
-        <f t="shared" si="70"/>
-        <v>110</v>
-      </c>
-      <c r="DJ33" s="6">
-        <f t="shared" si="71"/>
-        <v>111</v>
-      </c>
-      <c r="DK33" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="103:115" x14ac:dyDescent="0.35">
-      <c r="CY34" s="1">
-        <v>112</v>
-      </c>
-      <c r="CZ34" s="1">
-        <v>3</v>
-      </c>
-      <c r="DA34" s="3">
-        <v>0</v>
-      </c>
-      <c r="DB34" s="4"/>
-      <c r="DC34" s="4"/>
-      <c r="DD34" s="4"/>
-      <c r="DE34" s="5">
-        <f t="shared" si="69"/>
-        <v>0</v>
-      </c>
-      <c r="DF34" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG34" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH34" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI34" s="6">
-        <f t="shared" si="70"/>
-        <v>1</v>
-      </c>
-      <c r="DJ34" s="6">
-        <f t="shared" si="71"/>
-        <v>3</v>
-      </c>
-      <c r="DK34" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="103:115" x14ac:dyDescent="0.35">
-      <c r="CY35" s="1">
-        <v>113</v>
-      </c>
-      <c r="CZ35" s="1">
-        <v>6</v>
-      </c>
-      <c r="DA35" s="3">
-        <v>110</v>
-      </c>
-      <c r="DB35" s="4">
-        <v>112</v>
-      </c>
-      <c r="DC35" s="4"/>
-      <c r="DD35" s="4"/>
-      <c r="DE35" s="5">
-        <f t="shared" si="69"/>
-        <v>116</v>
-      </c>
-      <c r="DF35" s="5">
-        <f t="shared" si="66"/>
-        <v>3</v>
-      </c>
-      <c r="DG35" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH35" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI35" s="6">
-        <f t="shared" si="70"/>
-        <v>113</v>
-      </c>
-      <c r="DJ35" s="6">
-        <f t="shared" si="71"/>
-        <v>118</v>
-      </c>
-      <c r="DK35" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="103:115" x14ac:dyDescent="0.35">
-      <c r="CY36" s="1">
-        <v>114</v>
-      </c>
-      <c r="CZ36" s="1">
-        <v>7</v>
-      </c>
-      <c r="DA36" s="3">
-        <v>111</v>
-      </c>
-      <c r="DB36" s="4">
-        <v>115</v>
-      </c>
-      <c r="DC36" s="4"/>
-      <c r="DD36" s="4"/>
-      <c r="DE36" s="5">
-        <f t="shared" si="69"/>
-        <v>111</v>
-      </c>
-      <c r="DF36" s="5">
-        <f t="shared" si="66"/>
-        <v>112</v>
-      </c>
-      <c r="DG36" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH36" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI36" s="6">
-        <f t="shared" si="70"/>
-        <v>116</v>
-      </c>
-      <c r="DJ36" s="6">
-        <f t="shared" si="71"/>
-        <v>122</v>
-      </c>
-      <c r="DK36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="103:115" x14ac:dyDescent="0.35">
-      <c r="CY37" s="1">
-        <v>115</v>
-      </c>
-      <c r="CZ37" s="1">
-        <v>3</v>
-      </c>
-      <c r="DA37" s="3">
-        <v>109</v>
-      </c>
-      <c r="DB37" s="4"/>
-      <c r="DC37" s="4"/>
-      <c r="DD37" s="4"/>
-      <c r="DE37" s="5">
-        <f t="shared" si="69"/>
-        <v>116</v>
-      </c>
-      <c r="DF37" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG37" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH37" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI37" s="6">
-        <f t="shared" si="70"/>
-        <v>110</v>
-      </c>
-      <c r="DJ37" s="6">
-        <f t="shared" si="71"/>
-        <v>112</v>
-      </c>
-      <c r="DK37" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="103:115" x14ac:dyDescent="0.35">
-      <c r="CY38" s="1">
-        <v>116</v>
-      </c>
-      <c r="CZ38" s="1">
-        <v>6</v>
-      </c>
-      <c r="DA38" s="3">
-        <v>0</v>
-      </c>
-      <c r="DB38" s="4"/>
-      <c r="DC38" s="4"/>
-      <c r="DD38" s="4"/>
-      <c r="DE38" s="5">
-        <f t="shared" si="69"/>
-        <v>0</v>
-      </c>
-      <c r="DF38" s="5">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="DG38" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH38" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI38" s="6">
-        <f t="shared" si="70"/>
-        <v>1</v>
-      </c>
-      <c r="DJ38" s="6">
-        <f t="shared" si="71"/>
-        <v>6</v>
-      </c>
-      <c r="DK38" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="103:115" x14ac:dyDescent="0.35">
-      <c r="CY39" s="1">
-        <v>117</v>
-      </c>
-      <c r="CZ39" s="1">
-        <v>9</v>
-      </c>
-      <c r="DA39" s="3">
-        <v>114</v>
-      </c>
-      <c r="DB39" s="4">
-        <v>116</v>
-      </c>
-      <c r="DC39" s="4"/>
-      <c r="DD39" s="4"/>
-      <c r="DE39" s="5">
-        <f t="shared" si="69"/>
-        <v>122</v>
-      </c>
-      <c r="DF39" s="5">
-        <f t="shared" si="66"/>
-        <v>6</v>
-      </c>
-      <c r="DG39" s="5">
-        <f t="shared" si="67"/>
-        <v>0</v>
-      </c>
-      <c r="DH39" s="5">
-        <f t="shared" si="68"/>
-        <v>0</v>
-      </c>
-      <c r="DI39" s="6">
-        <f t="shared" si="70"/>
-        <v>117</v>
-      </c>
-      <c r="DJ39" s="6">
-        <f t="shared" si="71"/>
-        <v>125</v>
-      </c>
-      <c r="DK39" s="7">
         <v>0</v>
       </c>
     </row>

</xml_diff>